<commit_message>
Use https://github.com/protobi/js-xlsx/tree/beta to read color directly from xlsx
</commit_message>
<xml_diff>
--- a/www/input/corrplot.xlsx
+++ b/www/input/corrplot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bzhang1/github/quickr/www/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231E84A4-8D15-714F-96A8-71AB1DBF465B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AA5E47-533F-D146-A9C7-9B66369E1AB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32920" yWindow="7000" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="12520" windowWidth="32280" windowHeight="18580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -155,20 +155,20 @@
     <t>color.ramp.palette</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>Tropic</t>
   </si>
   <si>
     <t>Green-Orange</t>
+  </si>
+  <si>
+    <t>Custom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -303,6 +303,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="48">
     <fill>
@@ -486,36 +491,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBF3F45"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2978A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF70ABDA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF3B78A7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF019C9F"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -571,6 +546,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF4952B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4477AA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF77AADD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEE9988"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBB4444"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,7 +740,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -747,6 +752,7 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
@@ -801,16 +807,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBB4444"/>
+      <color rgb="FFEE9988"/>
+      <color rgb="FFFFFFFF"/>
+      <color rgb="FF77AADD"/>
+      <color rgb="FF4477AA"/>
       <color rgb="FFF4952B"/>
       <color rgb="FFF3BB98"/>
       <color rgb="FFE2E2E2"/>
       <color rgb="FF94D69F"/>
       <color rgb="FF00C74B"/>
-      <color rgb="FFC95BA7"/>
-      <color rgb="FFDFA8CA"/>
-      <color rgb="FFF1F1F1"/>
-      <color rgb="FF78C6C7"/>
-      <color rgb="FF019C9F"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1124,12 +1130,12 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1202,7 +1208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1240,7 +1246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1278,7 +1284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1316,7 +1322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1354,7 +1360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1392,7 +1398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1430,7 +1436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1468,7 +1474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1506,7 +1512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1582,7 +1588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1620,7 +1626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1658,7 +1664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1696,7 +1702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1734,7 +1740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1772,7 +1778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1810,7 +1816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1848,7 +1854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1886,7 +1892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1924,7 +1930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1962,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -2000,7 +2006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -2038,7 +2044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -2076,7 +2082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2114,7 +2120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -2152,7 +2158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -2190,7 +2196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -2228,7 +2234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -2266,7 +2272,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -2304,7 +2310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -2342,7 +2348,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -2390,56 +2396,56 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>43</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
-      <c r="I1" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
-      <c r="I2" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="D3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
-      <c r="I3" t="s">
-        <v>46</v>
-      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{A7FA9B97-91D5-4746-BD32-EBA8E618E939}">
-      <formula1>$I$1:$I$3</formula1>
+      <formula1>$D$1:$D$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>